<commit_message>
changed the xlsx files and wrote the pyhton script from scratch
</commit_message>
<xml_diff>
--- a/data/Food_nutrition_Intake/food_table2.xlsx
+++ b/data/Food_nutrition_Intake/food_table2.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20201077\Desktop\DorukGüngör\Eindhoven\Data_Science_AI\Knowledge_Engineering\Knowledge-Engineering-2AMD20-\data\Food_nutrition_Intake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057151FF-FE1F-425D-B853-496AA2722365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B4D05A-0943-4BF4-AEAF-5F269C16FE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Food density 2015 2016" sheetId="1" r:id="rId1"/>
-    <sheet name="Food density 2017 2018" sheetId="2" r:id="rId2"/>
+    <sheet name="2015 2016" sheetId="1" r:id="rId1"/>
+    <sheet name="2017 2018" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -1895,7 +1895,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
@@ -2023,7 +2023,7 @@
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
     </row>
-    <row r="35" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>31</v>
       </c>
@@ -2293,7 +2293,7 @@
       <c r="G46" s="21"/>
       <c r="H46" s="21"/>
     </row>
-    <row r="47" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
         <v>31</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>2.34</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>30</v>
       </c>
@@ -2652,8 +2652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD88872C-272C-40CF-8C86-2CA72B4E2B52}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O51" sqref="O51"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2752,7 +2752,7 @@
         <v>15.07</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>17.93</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>10.16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>30</v>
       </c>
@@ -3330,7 +3330,7 @@
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
         <v>31</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
@@ -3420,7 +3420,7 @@
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
         <v>31</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>30</v>
       </c>
@@ -3510,7 +3510,7 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
         <v>31</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>30</v>
       </c>
@@ -3600,7 +3600,7 @@
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
         <v>31</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>30</v>
       </c>
@@ -3690,7 +3690,7 @@
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
         <v>31</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>30</v>
       </c>
@@ -3780,7 +3780,7 @@
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
     </row>
-    <row r="51" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
         <v>31</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>30</v>
       </c>
@@ -3870,7 +3870,7 @@
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="20" t="s">
         <v>31</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>1.46</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>30</v>
       </c>

</xml_diff>